<commit_message>
code cleanup, add axisymmetric example
</commit_message>
<xml_diff>
--- a/tests/inputfiles/UX_2D.xlsx
+++ b/tests/inputfiles/UX_2D.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74927A41-6D99-4934-B073-D1AB8680012B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB45ED79-684E-45FE-B4AA-9623DD99ED10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="720" windowWidth="15885" windowHeight="11610" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Forces" sheetId="3" r:id="rId5"/>
     <sheet name="ControlledDOF" sheetId="7" r:id="rId6"/>
     <sheet name="BoundaryConditions" sheetId="9" r:id="rId7"/>
+    <sheet name="Loadcases" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>x</t>
   </si>
@@ -34,9 +35,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>Quad4</t>
-  </si>
-  <si>
     <t>Fx</t>
   </si>
   <si>
@@ -49,18 +47,12 @@
     <t>Connectivity</t>
   </si>
   <si>
-    <t>Parameters</t>
-  </si>
-  <si>
     <t>Material</t>
   </si>
   <si>
     <t>Label</t>
   </si>
   <si>
-    <t>Steel</t>
-  </si>
-  <si>
     <t>Rubber</t>
   </si>
   <si>
@@ -98,6 +90,39 @@
   </si>
   <si>
     <t>f0</t>
+  </si>
+  <si>
+    <t>Quad4p</t>
+  </si>
+  <si>
+    <t>multi-k</t>
+  </si>
+  <si>
+    <t>Tolerance</t>
+  </si>
+  <si>
+    <t>Iterations</t>
+  </si>
+  <si>
+    <t>Increments</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Loadcase1</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -129,9 +154,33 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -141,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -151,9 +200,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -167,6 +213,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -453,23 +506,23 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="1" max="3" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -480,7 +533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -491,7 +544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -502,7 +555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -523,42 +576,42 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="6" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.3828125" style="1"/>
+    <col min="2" max="2" width="12.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.15234375" style="5" customWidth="1"/>
+    <col min="4" max="5" width="11.3828125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>6</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5">
         <v>0</v>
       </c>
       <c r="D2" s="1">
@@ -574,15 +627,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
@@ -593,54 +646,70 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="13.3046875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.3828125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5">
         <v>5000</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="E5" s="1"/>
     </row>
   </sheetData>
@@ -656,58 +725,58 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="7"/>
-      <c r="I1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -722,21 +791,21 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
       <c r="B2" s="3">
@@ -746,8 +815,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="3">
@@ -757,49 +826,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -814,92 +883,92 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>13</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" s="4">
         <v>0</v>
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -913,49 +982,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1590A08E-9CDC-452D-9BA7-86A72CD84817}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="6">
-        <v>10</v>
+      <c r="B3" s="5">
+        <v>0.1</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2167F238-2B38-4FEC-B803-2359656D4903}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="10">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>